<commit_message>
Updated Global tests to use main objects/new grid.
</commit_message>
<xml_diff>
--- a/Accounting/Create Tax Product/Main.rvl.xlsx
+++ b/Accounting/Create Tax Product/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="120">
   <si>
     <t>Flow</t>
   </si>
@@ -346,6 +346,33 @@
   </si>
   <si>
     <t>TUXr A/R</t>
+  </si>
+  <si>
+    <t>UX_Grid</t>
+  </si>
+  <si>
+    <t>****Test searches for each tax rate in the SetupData spreadsheet.</t>
+  </si>
+  <si>
+    <t>*****If Tax Rate exists, do not create the Tax Rate setup.</t>
+  </si>
+  <si>
+    <t>******If Tax Rate doesn't exist, create Tax Rate using data from the spreadsheet.</t>
+  </si>
+  <si>
+    <t>****Test first searches if TUXr Tax product exists.</t>
+  </si>
+  <si>
+    <t>*****If Tax Rate exists, do not create the Tax Product setup.</t>
+  </si>
+  <si>
+    <t>*****If Tax Product exists, do not create the Tax Product setup.</t>
+  </si>
+  <si>
+    <t>******If Tax Product doesn't exist, create Tax Product.</t>
+  </si>
+  <si>
+    <t>Check if tax product already exists.</t>
   </si>
 </sst>
 </file>
@@ -366,7 +393,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="223">
+  <borders count="230">
     <border>
       <left/>
       <right/>
@@ -596,11 +623,18 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -824,6 +858,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="220" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="222" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="223" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="224" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="226" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="227" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="228" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -833,7 +874,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:H79"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5546875" customWidth="true"/>
@@ -900,432 +941,408 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="163"/>
+      <c r="A4" s="227"/>
     </row>
     <row r="5">
-      <c r="A5" s="162" t="s">
+      <c r="A5" s="226"/>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="225"/>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="224"/>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="223"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="163"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="162" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E10" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F10" t="s">
         <v>19</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="161"/>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="11">
+      <c r="A11" s="161"/>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F11" t="s">
         <v>22</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="174" t="s">
+    <row r="12">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="174" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="173"/>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="14">
+      <c r="A14" s="173"/>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D14" t="s">
         <v>26</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E14" t="s">
         <v>27</v>
       </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="172"/>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="172"/>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D15" t="s">
         <v>30</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E15" t="s">
         <v>31</v>
       </c>
-      <c r="F10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="171"/>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
+    <row r="16">
+      <c r="A16" s="171"/>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
         <v>29</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E16" t="s">
         <v>34</v>
       </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="170"/>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="17">
+      <c r="A17" s="170"/>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
         <v>29</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D17" t="s">
         <v>36</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E17" t="s">
         <v>31</v>
       </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="169"/>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="18">
+      <c r="A18" s="169"/>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
         <v>29</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E18" t="s">
         <v>39</v>
       </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="168"/>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="19">
+      <c r="A19" s="168"/>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
         <v>9</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D19" t="s">
         <v>41</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E19" t="s">
         <v>42</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F19" t="s">
         <v>43</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="167"/>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="20">
+      <c r="A20" s="167"/>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" t="s">
         <v>46</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E20" t="s">
         <v>47</v>
       </c>
-      <c r="F15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="166"/>
-      <c r="B16" t="s">
+    <row r="21">
+      <c r="A21" s="166"/>
+      <c r="B21" t="s">
         <v>11</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E21" t="s">
         <v>48</v>
       </c>
-      <c r="F16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18" t="s">
+    <row r="22">
+      <c r="A22" s="17"/>
+      <c r="B22" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21" t="s">
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="23" t="s">
+      <c r="F22" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="24"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="184" t="s">
+      <c r="H22" s="24"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="184" t="s">
         <v>55</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B23" t="s">
         <v>11</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E23" t="s">
         <v>56</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F23" t="s">
         <v>19</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="183"/>
-      <c r="B19" t="s">
+    <row r="24">
+      <c r="A24" s="183"/>
+      <c r="B24" t="s">
         <v>58</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D24" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="182" t="s">
+    <row r="25">
+      <c r="A25" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="181"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="180" t="s">
+    <row r="26">
+      <c r="A26" s="181"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B27" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="221"/>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
+    <row r="28">
+      <c r="A28" s="221"/>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
         <v>25</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D28" t="s">
         <v>26</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E28" t="s">
         <v>27</v>
       </c>
-      <c r="F23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="220"/>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s">
+    <row r="29">
+      <c r="A29" s="220"/>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
         <v>29</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D29" t="s">
         <v>64</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E29" t="s">
         <v>65</v>
       </c>
-      <c r="F24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="219"/>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="218"/>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="217"/>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="216"/>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="215"/>
-      <c r="B29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" t="s">
-        <v>75</v>
-      </c>
-    </row>
     <row r="30">
-      <c r="A30" s="214"/>
+      <c r="A30" s="219"/>
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -1333,7 +1350,7 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E30" t="s">
         <v>67</v>
@@ -1342,11 +1359,11 @@
         <v>22</v>
       </c>
       <c r="G30" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="213"/>
+      <c r="A31" s="218"/>
       <c r="B31" t="s">
         <v>11</v>
       </c>
@@ -1357,95 +1374,104 @@
         <v>13</v>
       </c>
       <c r="G31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="217"/>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="216"/>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="215"/>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="212"/>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
+    <row r="35">
+      <c r="A35" s="214"/>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
         <v>29</v>
       </c>
-      <c r="D32" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" t="s">
         <v>67</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F35" t="s">
         <v>22</v>
       </c>
-      <c r="G32" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="211"/>
-      <c r="B33" t="s">
+      <c r="G35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="213"/>
+      <c r="B36" t="s">
         <v>11</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E36" t="s">
         <v>39</v>
       </c>
-      <c r="F33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="210"/>
-      <c r="B34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" t="s">
-        <v>22</v>
-      </c>
-      <c r="G34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="209"/>
-      <c r="B35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" t="s">
-        <v>39</v>
-      </c>
-      <c r="F35" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="208"/>
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" t="s">
-        <v>82</v>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="207"/>
+      <c r="A37" s="212"/>
       <c r="B37" t="s">
         <v>3</v>
       </c>
@@ -1453,41 +1479,35 @@
         <v>29</v>
       </c>
       <c r="D37" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="E37" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="F37" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="G37" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="206"/>
+      <c r="A38" s="211"/>
       <c r="B38" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="F38" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="205"/>
+      <c r="A39" s="210"/>
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -1504,11 +1524,11 @@
         <v>22</v>
       </c>
       <c r="G39" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="204"/>
+      <c r="A40" s="209"/>
       <c r="B40" t="s">
         <v>11</v>
       </c>
@@ -1519,47 +1539,44 @@
         <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="203"/>
+      <c r="A41" s="208"/>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="207"/>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
         <v>29</v>
       </c>
-      <c r="D41" t="s">
-        <v>73</v>
-      </c>
-      <c r="E41" t="s">
-        <v>67</v>
-      </c>
-      <c r="F41" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="202"/>
-      <c r="B42" t="s">
-        <v>11</v>
+      <c r="D42" t="s">
+        <v>83</v>
       </c>
       <c r="E42" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="F42" t="s">
         <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="201"/>
+      <c r="A43" s="206"/>
       <c r="B43" t="s">
         <v>3</v>
       </c>
@@ -1567,7 +1584,7 @@
         <v>29</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="E43" t="s">
         <v>67</v>
@@ -1576,58 +1593,83 @@
         <v>22</v>
       </c>
       <c r="G43" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="200"/>
+      <c r="A44" s="205"/>
       <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="204"/>
+      <c r="B45" t="s">
         <v>11</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>39</v>
       </c>
-      <c r="F44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="198"/>
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="203"/>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
         <v>29</v>
       </c>
-      <c r="D45" t="s">
-        <v>64</v>
-      </c>
-      <c r="E45" t="s">
-        <v>31</v>
-      </c>
-      <c r="F45" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="197"/>
+      <c r="D46" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F46" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="196" t="s">
-        <v>15</v>
-      </c>
+      <c r="A47" s="202"/>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>11</v>
+      </c>
+      <c r="E47" t="s">
+        <v>39</v>
+      </c>
+      <c r="F47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="195"/>
+      <c r="A48" s="201"/>
       <c r="B48" t="s">
         <v>3</v>
       </c>
@@ -1635,41 +1677,35 @@
         <v>29</v>
       </c>
       <c r="D48" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="E48" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="F48" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="G48" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="194"/>
+      <c r="A49" s="200"/>
       <c r="B49" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" t="s">
-        <v>29</v>
-      </c>
-      <c r="D49" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F49" t="s">
         <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="193"/>
+      <c r="A50" s="198"/>
       <c r="B50" t="s">
         <v>3</v>
       </c>
@@ -1677,7 +1713,7 @@
         <v>29</v>
       </c>
       <c r="D50" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="E50" t="s">
         <v>31</v>
@@ -1686,104 +1722,85 @@
         <v>13</v>
       </c>
       <c r="G50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="197"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="196" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="195"/>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" t="s">
+        <v>31</v>
+      </c>
+      <c r="F53" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="194"/>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="193"/>
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55" t="s">
+        <v>36</v>
+      </c>
+      <c r="E55" t="s">
+        <v>31</v>
+      </c>
+      <c r="F55" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="192"/>
-      <c r="B51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" t="s">
-        <v>29</v>
-      </c>
-      <c r="D51" t="s">
-        <v>38</v>
-      </c>
-      <c r="E51" t="s">
-        <v>39</v>
-      </c>
-      <c r="F51" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="191"/>
-      <c r="B52" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" t="s">
-        <v>41</v>
-      </c>
-      <c r="E52" t="s">
-        <v>42</v>
-      </c>
-      <c r="F52" t="s">
-        <v>43</v>
-      </c>
-      <c r="G52" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="190"/>
-      <c r="B53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C53" t="s">
-        <v>45</v>
-      </c>
-      <c r="D53" t="s">
-        <v>97</v>
-      </c>
-      <c r="E53" t="s">
-        <v>47</v>
-      </c>
-      <c r="F53" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="189"/>
-      <c r="B54" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" t="s">
-        <v>48</v>
-      </c>
-      <c r="F54" t="s">
-        <v>13</v>
-      </c>
-      <c r="G54" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="222"/>
-      <c r="B55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" t="s">
-        <v>52</v>
-      </c>
-      <c r="F55" t="s">
-        <v>13</v>
-      </c>
-      <c r="G55" t="s">
-        <v>54</v>
-      </c>
-    </row>
     <row r="56">
-      <c r="A56" s="188"/>
+      <c r="A56" s="192"/>
       <c r="B56" t="s">
         <v>3</v>
       </c>
@@ -1791,40 +1808,52 @@
         <v>29</v>
       </c>
       <c r="D56" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="E56" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="F56" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G56" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="187"/>
+      <c r="A57" s="191"/>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" t="s">
+        <v>41</v>
       </c>
       <c r="E57" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="F57" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="G57" t="s">
-        <v>101</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="186"/>
+      <c r="A58" s="190"/>
       <c r="B58" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="C58" t="s">
+        <v>111</v>
+      </c>
+      <c r="D58" t="s">
+        <v>97</v>
       </c>
       <c r="E58" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="F58" t="s">
         <v>13</v>
@@ -1834,179 +1863,230 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="185" t="s">
+      <c r="A59" s="189"/>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
+        <v>48</v>
+      </c>
+      <c r="F59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="222"/>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
+        <v>52</v>
+      </c>
+      <c r="F60" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="188"/>
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61" t="s">
+        <v>98</v>
+      </c>
+      <c r="E61" t="s">
+        <v>102</v>
+      </c>
+      <c r="F61" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="185" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" s="25"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="31"/>
-      <c r="H60" s="32"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="33"/>
-      <c r="B61" s="34"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="38"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="40"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="41"/>
-      <c r="B62" s="42"/>
-      <c r="C62" s="43"/>
-      <c r="D62" s="44"/>
-      <c r="E62" s="45"/>
-      <c r="F62" s="46"/>
-      <c r="G62" s="47"/>
-      <c r="H62" s="48"/>
-    </row>
     <row r="63">
-      <c r="A63" s="49"/>
-      <c r="B63" s="50"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="52"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="54"/>
-      <c r="G63" s="55"/>
-      <c r="H63" s="56"/>
+      <c r="A63" s="25"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="31"/>
+      <c r="H63" s="32"/>
     </row>
     <row r="64">
-      <c r="A64" s="57"/>
-      <c r="B64" s="58"/>
-      <c r="C64" s="59"/>
-      <c r="D64" s="60"/>
-      <c r="E64" s="61"/>
-      <c r="F64" s="62"/>
-      <c r="G64" s="63"/>
-      <c r="H64" s="64"/>
+      <c r="A64" s="33"/>
+      <c r="B64" s="34"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="40"/>
     </row>
     <row r="65">
-      <c r="A65" s="65"/>
-      <c r="B65" s="66"/>
-      <c r="C65" s="67"/>
-      <c r="D65" s="68"/>
-      <c r="E65" s="69"/>
-      <c r="F65" s="70"/>
-      <c r="G65" s="71"/>
-      <c r="H65" s="72"/>
+      <c r="A65" s="41"/>
+      <c r="B65" s="42"/>
+      <c r="C65" s="43"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="46"/>
+      <c r="G65" s="47"/>
+      <c r="H65" s="48"/>
     </row>
     <row r="66">
-      <c r="A66" s="73"/>
-      <c r="B66" s="74"/>
-      <c r="C66" s="75"/>
-      <c r="D66" s="76"/>
-      <c r="E66" s="77"/>
-      <c r="F66" s="78"/>
-      <c r="G66" s="79"/>
-      <c r="H66" s="80"/>
+      <c r="A66" s="49"/>
+      <c r="B66" s="50"/>
+      <c r="C66" s="51"/>
+      <c r="D66" s="52"/>
+      <c r="E66" s="53"/>
+      <c r="F66" s="54"/>
+      <c r="G66" s="55"/>
+      <c r="H66" s="56"/>
     </row>
     <row r="67">
-      <c r="A67" s="81"/>
-      <c r="B67" s="82"/>
-      <c r="C67" s="83"/>
-      <c r="D67" s="84"/>
-      <c r="E67" s="85"/>
-      <c r="F67" s="86"/>
-      <c r="G67" s="87"/>
-      <c r="H67" s="88"/>
+      <c r="A67" s="57"/>
+      <c r="B67" s="58"/>
+      <c r="C67" s="59"/>
+      <c r="D67" s="60"/>
+      <c r="E67" s="61"/>
+      <c r="F67" s="62"/>
+      <c r="G67" s="63"/>
+      <c r="H67" s="64"/>
     </row>
     <row r="68">
-      <c r="A68" s="89"/>
-      <c r="B68" s="90"/>
-      <c r="C68" s="91"/>
-      <c r="D68" s="92"/>
-      <c r="E68" s="93"/>
-      <c r="F68" s="94"/>
-      <c r="G68" s="95"/>
-      <c r="H68" s="96"/>
+      <c r="A68" s="65"/>
+      <c r="B68" s="66"/>
+      <c r="C68" s="67"/>
+      <c r="D68" s="68"/>
+      <c r="E68" s="69"/>
+      <c r="F68" s="70"/>
+      <c r="G68" s="71"/>
+      <c r="H68" s="72"/>
     </row>
     <row r="69">
-      <c r="A69" s="97"/>
-      <c r="B69" s="98"/>
-      <c r="C69" s="99"/>
-      <c r="D69" s="100"/>
-      <c r="E69" s="101"/>
-      <c r="F69" s="102"/>
-      <c r="G69" s="103"/>
-      <c r="H69" s="104"/>
+      <c r="A69" s="73"/>
+      <c r="B69" s="74"/>
+      <c r="C69" s="75"/>
+      <c r="D69" s="76"/>
+      <c r="E69" s="77"/>
+      <c r="F69" s="78"/>
+      <c r="G69" s="79"/>
+      <c r="H69" s="80"/>
     </row>
     <row r="70">
-      <c r="A70" s="105"/>
-      <c r="B70" s="106"/>
-      <c r="C70" s="107"/>
-      <c r="D70" s="108"/>
-      <c r="E70" s="109"/>
-      <c r="F70" s="110"/>
-      <c r="G70" s="111"/>
-      <c r="H70" s="112"/>
+      <c r="A70" s="81"/>
+      <c r="B70" s="82"/>
+      <c r="C70" s="83"/>
+      <c r="D70" s="84"/>
+      <c r="E70" s="85"/>
+      <c r="F70" s="86"/>
+      <c r="G70" s="87"/>
+      <c r="H70" s="88"/>
     </row>
     <row r="71">
-      <c r="A71" s="113"/>
-      <c r="B71" s="114"/>
-      <c r="C71" s="115"/>
-      <c r="D71" s="116"/>
-      <c r="E71" s="117"/>
-      <c r="F71" s="118"/>
-      <c r="G71" s="119"/>
-      <c r="H71" s="120"/>
+      <c r="A71" s="89"/>
+      <c r="B71" s="90"/>
+      <c r="C71" s="91"/>
+      <c r="D71" s="92"/>
+      <c r="E71" s="93"/>
+      <c r="F71" s="94"/>
+      <c r="G71" s="95"/>
+      <c r="H71" s="96"/>
     </row>
     <row r="72">
-      <c r="A72" s="121"/>
-      <c r="B72" s="122"/>
-      <c r="C72" s="123"/>
-      <c r="D72" s="124"/>
-      <c r="E72" s="125"/>
-      <c r="F72" s="126"/>
-      <c r="G72" s="127"/>
-      <c r="H72" s="128"/>
+      <c r="A72" s="97"/>
+      <c r="B72" s="98"/>
+      <c r="C72" s="99"/>
+      <c r="D72" s="100"/>
+      <c r="E72" s="101"/>
+      <c r="F72" s="102"/>
+      <c r="G72" s="103"/>
+      <c r="H72" s="104"/>
     </row>
     <row r="73">
-      <c r="A73" s="129"/>
-      <c r="B73" s="130"/>
-      <c r="C73" s="131"/>
-      <c r="D73" s="132"/>
-      <c r="E73" s="133"/>
-      <c r="F73" s="134"/>
-      <c r="G73" s="135"/>
-      <c r="H73" s="136"/>
+      <c r="A73" s="105"/>
+      <c r="B73" s="106"/>
+      <c r="C73" s="107"/>
+      <c r="D73" s="108"/>
+      <c r="E73" s="109"/>
+      <c r="F73" s="110"/>
+      <c r="G73" s="111"/>
+      <c r="H73" s="112"/>
     </row>
     <row r="74">
-      <c r="A74" s="137"/>
-      <c r="B74" s="138"/>
-      <c r="C74" s="139"/>
-      <c r="D74" s="140"/>
-      <c r="E74" s="141"/>
-      <c r="F74" s="142"/>
-      <c r="G74" s="143"/>
-      <c r="H74" s="144"/>
+      <c r="A74" s="113"/>
+      <c r="B74" s="114"/>
+      <c r="C74" s="115"/>
+      <c r="D74" s="116"/>
+      <c r="E74" s="117"/>
+      <c r="F74" s="118"/>
+      <c r="G74" s="119"/>
+      <c r="H74" s="120"/>
     </row>
     <row r="75">
-      <c r="A75" s="145"/>
-      <c r="B75" s="146"/>
-      <c r="C75" s="147"/>
-      <c r="D75" s="148"/>
-      <c r="E75" s="149"/>
-      <c r="F75" s="150"/>
-      <c r="G75" s="151"/>
-      <c r="H75" s="152"/>
+      <c r="A75" s="121"/>
+      <c r="B75" s="122"/>
+      <c r="C75" s="123"/>
+      <c r="D75" s="124"/>
+      <c r="E75" s="125"/>
+      <c r="F75" s="126"/>
+      <c r="G75" s="127"/>
+      <c r="H75" s="128"/>
     </row>
     <row r="76">
-      <c r="A76" s="153"/>
-      <c r="B76" s="154"/>
-      <c r="C76" s="155"/>
-      <c r="D76" s="156"/>
-      <c r="E76" s="157"/>
-      <c r="F76" s="158"/>
-      <c r="G76" s="159"/>
-      <c r="H76" s="160"/>
+      <c r="A76" s="129"/>
+      <c r="B76" s="130"/>
+      <c r="C76" s="131"/>
+      <c r="D76" s="132"/>
+      <c r="E76" s="133"/>
+      <c r="F76" s="134"/>
+      <c r="G76" s="135"/>
+      <c r="H76" s="136"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="137"/>
+      <c r="B77" s="138"/>
+      <c r="C77" s="139"/>
+      <c r="D77" s="140"/>
+      <c r="E77" s="141"/>
+      <c r="F77" s="142"/>
+      <c r="G77" s="143"/>
+      <c r="H77" s="144"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="145"/>
+      <c r="B78" s="146"/>
+      <c r="C78" s="147"/>
+      <c r="D78" s="148"/>
+      <c r="E78" s="149"/>
+      <c r="F78" s="150"/>
+      <c r="G78" s="151"/>
+      <c r="H78" s="152"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="153"/>
+      <c r="B79" s="154"/>
+      <c r="C79" s="155"/>
+      <c r="D79" s="156"/>
+      <c r="E79" s="157"/>
+      <c r="F79" s="158"/>
+      <c r="G79" s="159"/>
+      <c r="H79" s="160"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>